<commit_message>
changes ask per coach
</commit_message>
<xml_diff>
--- a/PFS.xlsx
+++ b/PFS.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -479,6 +479,42 @@
       <c r="A6" t="inlineStr">
         <is>
           <t>Air bnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Feria</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Expense</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Mercado</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Expense</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Netflix</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Expense</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes as per coach request
</commit_message>
<xml_diff>
--- a/PFS.xlsx
+++ b/PFS.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,7 +12,7 @@
     <sheet name="Expense and incomes" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -51,7 +52,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -420,7 +421,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -432,13 +433,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -450,81 +451,34 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Universidad</t>
+          <t>Carro</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Expense</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Quincena</t>
+          <t>Universidad</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Expense</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Carro</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Medico</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Air bnb</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Feria</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Expense</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Mercado</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Expense</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Netflix</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Expense</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Servicios profesionales</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
+          <t>Servicios Profesionales</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Income</t>
         </is>
@@ -541,13 +495,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -589,19 +543,19 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>24500</t>
+          <t>4500</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>15na de abril</t>
+          <t>Analisis de un sistema informatico</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Quincena</t>
+          <t>Servicios Profesionales</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -611,95 +565,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>35000</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Llantas</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Carro</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Expense</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>18900</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Alquiler</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Air bnb</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Income</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>15000</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Queso tierno</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Mercado</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Expense</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>3250</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Analisis de programa informatico</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Servicios profesionales</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Income</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>15000</t>
+          <t>45000</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement suggestion as per coach request
</commit_message>
<xml_diff>
--- a/PFS.xlsx
+++ b/PFS.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7270" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,7 +11,7 @@
     <sheet name="Expense and incomes" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -52,7 +51,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -421,7 +420,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -433,13 +432,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -447,11 +446,16 @@
           <t>Category</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Carro</t>
+          <t>Casa</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -475,12 +479,24 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Servicios Profesionales</t>
+          <t>Servicios_Profesionales</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>Income</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Feria</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Expense</t>
         </is>
       </c>
     </row>
@@ -495,13 +511,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="20.08984375" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="10.7265625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="7.7265625" bestFit="1" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -543,29 +564,51 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4500</t>
+          <t>47500</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Analisis de un sistema informatico</t>
+          <t>Tomate,Zanahoria,Culantro</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Servicios Profesionales</t>
+          <t>Feria</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Expense</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>analisis de un sistema informatico</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Servicios_Profesionales</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Income</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>45000</t>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1500</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changes done as per coach request
</commit_message>
<xml_diff>
--- a/PFS.xlsx
+++ b/PFS.xlsx
@@ -1,35 +1,101 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29311"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_2621BC7A6EF2E08C96D47C2E0475181C79C9FFC2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BFB6B78-EE08-4C33-955D-AB6EFD0C5677}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7270" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7270" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="category" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Expense and incomes" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="category" sheetId="2" r:id="rId2"/>
+    <sheet name="Expense and incomes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Casa</t>
+  </si>
+  <si>
+    <t>Expense</t>
+  </si>
+  <si>
+    <t>Universidad</t>
+  </si>
+  <si>
+    <t>Servicios_Profesionales</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Feria</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Matricula</t>
+  </si>
+  <si>
+    <t>47500</t>
+  </si>
+  <si>
+    <t>Tomate,Zanahoria,Culantro</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>analisis de un sistema informatico</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -48,80 +114,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -409,95 +416,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Category</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Casa</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Expense</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Universidad</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Expense</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Servicios_Profesionales</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Income</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Feria</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Expense</t>
-        </is>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -506,110 +481,74 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col width="20.08984375" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="10.7265625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="7.7265625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Detail</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Category</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Amount</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Matricula</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Universidad</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Expense</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>47500</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Tomate,Zanahoria,Culantro</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Feria</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Expense</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>analisis de un sistema informatico</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Servicios_Profesionales</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Income</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>